<commit_message>
Automate data pull, transform, and regression
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14204,56 +14204,38 @@
       <c r="L172" t="n">
         <v>5060</v>
       </c>
-      <c r="M172" t="inlineStr">
+      <c r="M172" t="n">
+        <v>0</v>
+      </c>
+      <c r="N172" t="n">
+        <v>1</v>
+      </c>
+      <c r="O172" t="inlineStr"/>
+      <c r="P172" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q172" t="n">
+        <v>1</v>
+      </c>
+      <c r="R172" t="inlineStr">
         <is>
           <t>NOT REPORTED</t>
         </is>
       </c>
-      <c r="N172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="O172" t="inlineStr"/>
-      <c r="P172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="Q172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="R172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="S172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="T172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="U172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="V172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="W172" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
+      <c r="S172" t="n">
+        <v>0</v>
+      </c>
+      <c r="T172" t="n">
+        <v>1</v>
+      </c>
+      <c r="U172" t="n">
+        <v>1</v>
+      </c>
+      <c r="V172" t="n">
+        <v>1</v>
+      </c>
+      <c r="W172" t="n">
+        <v>1</v>
       </c>
       <c r="X172" t="n">
         <v>0</v>
@@ -14304,56 +14286,38 @@
       <c r="L173" t="n">
         <v>5372</v>
       </c>
-      <c r="M173" t="inlineStr">
+      <c r="M173" t="n">
+        <v>0</v>
+      </c>
+      <c r="N173" t="n">
+        <v>1</v>
+      </c>
+      <c r="O173" t="inlineStr"/>
+      <c r="P173" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q173" t="n">
+        <v>1</v>
+      </c>
+      <c r="R173" t="inlineStr">
         <is>
           <t>NOT REPORTED</t>
         </is>
       </c>
-      <c r="N173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="O173" t="inlineStr"/>
-      <c r="P173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="Q173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="R173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="S173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="T173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="U173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="V173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="W173" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
+      <c r="S173" t="n">
+        <v>0</v>
+      </c>
+      <c r="T173" t="n">
+        <v>1</v>
+      </c>
+      <c r="U173" t="n">
+        <v>1</v>
+      </c>
+      <c r="V173" t="n">
+        <v>1</v>
+      </c>
+      <c r="W173" t="n">
+        <v>1</v>
       </c>
       <c r="X173" t="n">
         <v>0</v>
@@ -14564,56 +14528,38 @@
       <c r="L176" t="n">
         <v>6559</v>
       </c>
-      <c r="M176" t="inlineStr">
+      <c r="M176" t="n">
+        <v>1</v>
+      </c>
+      <c r="N176" t="n">
+        <v>1</v>
+      </c>
+      <c r="O176" t="inlineStr"/>
+      <c r="P176" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q176" t="n">
+        <v>1</v>
+      </c>
+      <c r="R176" t="inlineStr">
         <is>
           <t>NOT REPORTED</t>
         </is>
       </c>
-      <c r="N176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="O176" t="inlineStr"/>
-      <c r="P176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="Q176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="R176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="S176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="T176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="U176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="V176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
-      </c>
-      <c r="W176" t="inlineStr">
-        <is>
-          <t>NOT REPORTED</t>
-        </is>
+      <c r="S176" t="n">
+        <v>0</v>
+      </c>
+      <c r="T176" t="n">
+        <v>1</v>
+      </c>
+      <c r="U176" t="n">
+        <v>1</v>
+      </c>
+      <c r="V176" t="n">
+        <v>1</v>
+      </c>
+      <c r="W176" t="n">
+        <v>1</v>
       </c>
       <c r="X176" t="n">
         <v>0</v>
@@ -20187,10 +20133,8 @@
       <c r="M246" t="n">
         <v>1</v>
       </c>
-      <c r="N246" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
+      <c r="N246" t="n">
+        <v>0</v>
       </c>
       <c r="O246" t="inlineStr"/>
       <c r="P246" t="n">
@@ -29949,7 +29893,9 @@
       <c r="M368" t="n">
         <v>0</v>
       </c>
-      <c r="N368" t="inlineStr"/>
+      <c r="N368" t="n">
+        <v>1</v>
+      </c>
       <c r="O368" t="inlineStr"/>
       <c r="P368" t="n">
         <v>1</v>
@@ -30507,7 +30453,9 @@
       <c r="M375" t="n">
         <v>0</v>
       </c>
-      <c r="N375" t="inlineStr"/>
+      <c r="N375" t="n">
+        <v>0</v>
+      </c>
       <c r="O375" t="n">
         <v>1</v>
       </c>
@@ -40998,7 +40946,9 @@
       <c r="R506" t="n">
         <v>0</v>
       </c>
-      <c r="S506" t="inlineStr"/>
+      <c r="S506" t="n">
+        <v>0</v>
+      </c>
       <c r="T506" t="n">
         <v>0</v>
       </c>
@@ -61239,7 +61189,9 @@
       <c r="S759" t="n">
         <v>0</v>
       </c>
-      <c r="T759" t="inlineStr"/>
+      <c r="T759" t="n">
+        <v>1</v>
+      </c>
       <c r="U759" t="n">
         <v>1</v>
       </c>
@@ -66901,7 +66853,9 @@
       <c r="M830" t="n">
         <v>1</v>
       </c>
-      <c r="N830" t="inlineStr"/>
+      <c r="N830" t="n">
+        <v>1</v>
+      </c>
       <c r="O830" t="inlineStr"/>
       <c r="P830" t="n">
         <v>1</v>
@@ -67459,7 +67413,9 @@
       <c r="M837" t="n">
         <v>1</v>
       </c>
-      <c r="N837" t="inlineStr"/>
+      <c r="N837" t="n">
+        <v>1</v>
+      </c>
       <c r="O837" t="n">
         <v>1</v>
       </c>
@@ -84753,7 +84709,9 @@
       <c r="S1053" t="n">
         <v>0</v>
       </c>
-      <c r="T1053" t="inlineStr"/>
+      <c r="T1053" t="n">
+        <v>0</v>
+      </c>
       <c r="U1053" t="n">
         <v>0</v>
       </c>

</xml_diff>